<commit_message>
Update Human development index (HDI).xlsx
</commit_message>
<xml_diff>
--- a/lecture/Human development index (HDI).xlsx
+++ b/lecture/Human development index (HDI).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Python Course\Spring 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saeed Saffari\Documents\GitHub\alzahra-workshop-spr2021\lecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B701BFB0-C308-46EB-B9A8-07005370105E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F573EC75-AB2E-4B5E-B0C0-3F5BAC93065B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{59EAB0DD-746E-47BC-9681-5DFDA7FD1CDC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{59EAB0DD-746E-47BC-9681-5DFDA7FD1CDC}"/>
   </bookViews>
   <sheets>
     <sheet name="HDI_1" sheetId="1" r:id="rId1"/>
@@ -1248,11 +1248,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9B4EE6-86CB-4D6C-94E1-E4A57B5AF891}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,7 +2084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88152281-6CC1-44A9-9C99-957D3BE35826}">
   <dimension ref="A1:B190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>